<commit_message>
Excel data changed. APIpath in one place, initial set up to manage parking screen
</commit_message>
<xml_diff>
--- a/src/mocks/User_data.xlsx
+++ b/src/mocks/User_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>First Name</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>jj3@gmail.com</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>brain</t>
+  </si>
+  <si>
+    <t>nick</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,7 +446,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -446,12 +455,12 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>6074147509</v>
+        <v>6074247509</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -461,12 +470,12 @@
         <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>6074147509</v>
+        <v>6074167509</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -476,7 +485,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>6074147509</v>
+        <v>6073147509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>